<commit_message>
Added image to img folder
Added image of excel graph
</commit_message>
<xml_diff>
--- a/excel/penglings-data-excel.xlsx
+++ b/excel/penglings-data-excel.xlsx
@@ -92,7 +92,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,12 +107,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -220,18 +214,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>